<commit_message>
Updated Roadmap Post R1.4
</commit_message>
<xml_diff>
--- a/Documentation/Future Plans/MaxDuino Development Roadmap.xlsx
+++ b/Documentation/Future Plans/MaxDuino Development Roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Alan\Arduino\Arduino Sketches\GitHub\MaxDuino\Documentation\Future Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF913B-ABC7-46EC-99FF-B8E26E6ABA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE7ED2C-7F39-4095-826F-0DBE45E6E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B16E0DF9-CE6E-473D-A853-270CC3AD2790}"/>
   </bookViews>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="143">
   <si>
     <t>Section</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>single SM 2812B</t>
   </si>
   <si>
     <t>Up to 15</t>
@@ -569,6 +566,59 @@
   </si>
   <si>
     <t>Knock on effect for D3 (Thr DCC decoding pin.)</t>
+  </si>
+  <si>
+    <t>single SM 2812B + Ext</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>When addressing item 1 above I moved DCC decoding to a new pin.
+Turned out that new pin did not support required interrupts.</t>
+  </si>
+  <si>
+    <t>DCC Dcecoding failed test.</t>
+  </si>
+  <si>
+    <t>Use R1.1 PCB for DCC Decoding.</t>
+  </si>
+  <si>
+    <t>No DCC Decoding</t>
+  </si>
+  <si>
+    <t>Redesign SCH and PCB to put DE/RE pins on D2 and D5. Return DCC decoding to D3  pin.</t>
+  </si>
+  <si>
+    <t>Include in V1.3</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>Look</t>
+  </si>
+  <si>
+    <t>Ignore minor stencil items.</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Include in V1.4</t>
+  </si>
+  <si>
+    <t>New production of R1.3</t>
+  </si>
+  <si>
+    <t>New production of R1.4</t>
+  </si>
+  <si>
+    <t>Some manual stencil items on the PCB were not properly updated. (Revision number for one).</t>
+  </si>
+  <si>
+    <t>Fix stencil items in R1.4
+While doing this rearrange order of D3 and D4 header pins</t>
   </si>
 </sst>
 </file>
@@ -657,7 +707,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +792,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -1053,7 +1109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1129,7 +1185,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1188,46 +1243,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,11 +1261,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1259,6 +1272,61 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1397,14 +1465,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>124558</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>80597</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>168519</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>80596</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>15067</xdr:rowOff>
     </xdr:to>
@@ -1421,7 +1489,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5018943" y="0"/>
+          <a:off x="5238751" y="0"/>
           <a:ext cx="761999" cy="3869029"/>
           <a:chOff x="9869366" y="109904"/>
           <a:chExt cx="761999" cy="3869029"/>
@@ -1834,7 +1902,7 @@
   <dimension ref="A2:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,7 +1926,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="33">
         <v>1</v>
@@ -1866,174 +1934,176 @@
       <c r="F3" s="34">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36">
+      <c r="G3" s="105">
         <v>1.2</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="39">
+      <c r="H3" s="35">
+        <v>1.4</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="38">
         <v>2</v>
       </c>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="40"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="39"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="80" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="82">
+      <c r="B4" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91">
         <v>1</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="83">
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="93">
         <v>2</v>
       </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="74">
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="92">
         <v>3</v>
       </c>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="83">
+      <c r="N4" s="92"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="92"/>
+      <c r="Q4" s="93">
         <v>4</v>
       </c>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="74">
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="92">
         <v>5</v>
       </c>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="75"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="94"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="80" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="76">
+      <c r="B5" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="95">
         <v>2023</v>
       </c>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="78">
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="97">
         <v>2024</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="77">
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="96">
         <v>2025</v>
       </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="78">
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="97">
         <v>2026</v>
       </c>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
-      <c r="T5" s="78"/>
-      <c r="U5" s="77">
+      <c r="R5" s="97"/>
+      <c r="S5" s="97"/>
+      <c r="T5" s="97"/>
+      <c r="U5" s="96">
         <v>2027</v>
       </c>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="79"/>
+      <c r="V5" s="96"/>
+      <c r="W5" s="96"/>
+      <c r="X5" s="98"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="51" t="s">
+      <c r="M6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="51" t="s">
+      <c r="O6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="50" t="s">
+      <c r="P6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="51" t="s">
+      <c r="Q6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="51" t="s">
+      <c r="S6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="50" t="s">
+      <c r="T6" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="51" t="s">
+      <c r="U6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="50" t="s">
+      <c r="V6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="W6" s="51" t="s">
+      <c r="W6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="55" t="s">
+      <c r="X6" s="54" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2043,31 +2113,31 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="61"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
+        <v>105</v>
+      </c>
+      <c r="E7" s="69"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="59"/>
     </row>
     <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
@@ -2075,22 +2145,22 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="71"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="103"/>
       <c r="H8" s="32"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="94"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="29"/>
       <c r="M8" s="31"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="30"/>
       <c r="Q8" s="29"/>
       <c r="R8" s="29"/>
@@ -2107,24 +2177,24 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="71"/>
+        <v>118</v>
+      </c>
+      <c r="E9" s="70"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="103"/>
       <c r="H9" s="32"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="L9" s="94"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="29"/>
       <c r="M9" s="31"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
       <c r="P9" s="30"/>
       <c r="Q9" s="29"/>
       <c r="R9" s="29"/>
@@ -2141,22 +2211,22 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="71"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="103"/>
       <c r="H10" s="32"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="94"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="29"/>
       <c r="M10" s="31"/>
-      <c r="N10" s="94"/>
-      <c r="O10" s="94"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
       <c r="P10" s="30"/>
       <c r="Q10" s="29"/>
       <c r="R10" s="29"/>
@@ -2173,24 +2243,24 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="71"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="87" t="s">
-        <v>64</v>
+      <c r="G11" s="104" t="s">
+        <v>63</v>
       </c>
       <c r="H11" s="32"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="94"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="29"/>
       <c r="M11" s="31"/>
-      <c r="N11" s="94"/>
-      <c r="O11" s="94"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
       <c r="P11" s="30"/>
       <c r="Q11" s="29"/>
       <c r="R11" s="29"/>
@@ -2207,22 +2277,22 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="71"/>
+      <c r="E12" s="70"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="103"/>
       <c r="H12" s="32"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="94"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="29"/>
       <c r="M12" s="31"/>
-      <c r="N12" s="94"/>
-      <c r="O12" s="94"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
       <c r="P12" s="30"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29"/>
@@ -2239,24 +2309,24 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="71"/>
+        <v>126</v>
+      </c>
+      <c r="E13" s="70"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="87" t="s">
-        <v>64</v>
+      <c r="G13" s="104" t="s">
+        <v>63</v>
       </c>
       <c r="H13" s="32"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="94"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="29"/>
       <c r="M13" s="31"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="94"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
@@ -2273,22 +2343,22 @@
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="71"/>
+        <v>18</v>
+      </c>
+      <c r="E14" s="70"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="103"/>
       <c r="H14" s="32"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="94"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="31"/>
-      <c r="N14" s="94"/>
-      <c r="O14" s="94"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
       <c r="P14" s="30"/>
       <c r="Q14" s="29"/>
       <c r="R14" s="29"/>
@@ -2305,24 +2375,26 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="105" t="s">
-        <v>124</v>
+      <c r="E15" s="88" t="s">
+        <v>123</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="106" t="s">
+        <v>123</v>
+      </c>
       <c r="H15" s="32"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="94"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="31"/>
-      <c r="N15" s="94"/>
-      <c r="O15" s="94"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
       <c r="P15" s="30"/>
       <c r="Q15" s="29"/>
       <c r="R15" s="29"/>
@@ -2336,85 +2408,85 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E16" s="68"/>
+        <v>117</v>
+      </c>
+      <c r="E16" s="67"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="68"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="103" t="s">
-        <v>123</v>
-      </c>
-      <c r="L16" s="98"/>
-      <c r="M16" s="100"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="98"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="100"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="62"/>
+      <c r="K16" s="86" t="s">
+        <v>122</v>
+      </c>
+      <c r="L16" s="46"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="83"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="61"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="69"/>
+        <v>117</v>
+      </c>
+      <c r="E17" s="68"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="69"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="68"/>
       <c r="J17" s="19"/>
-      <c r="K17" s="104" t="s">
-        <v>123</v>
-      </c>
-      <c r="L17" s="99"/>
-      <c r="M17" s="101"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="102"/>
-      <c r="T17" s="102"/>
-      <c r="U17" s="101"/>
-      <c r="V17" s="102"/>
-      <c r="W17" s="102"/>
-      <c r="X17" s="48"/>
+      <c r="K17" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="82"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="85"/>
+      <c r="R17" s="85"/>
+      <c r="S17" s="85"/>
+      <c r="T17" s="85"/>
+      <c r="U17" s="84"/>
+      <c r="V17" s="85"/>
+      <c r="W17" s="85"/>
+      <c r="X17" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="U5:X5"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="Q4:T4"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="U5:X5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2439,75 +2511,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="84"/>
+      <c r="A1" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="99"/>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2558,7 +2630,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,89 +2646,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
+      <c r="A1" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="20"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="85" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="86" t="s">
-        <v>48</v>
+      <c r="G1" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="101" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="100"/>
+      <c r="H2" s="101"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="73">
+        <v>1</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="88">
-        <v>1</v>
-      </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="92">
+      <c r="G3" s="77">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="41">
+        <v>87</v>
+      </c>
+      <c r="G4" s="40">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2665,76 +2737,76 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="40">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="78">
+        <v>3</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="41">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="93">
-        <v>3</v>
-      </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="46" t="s">
+      <c r="E6" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="75">
+        <v>1.2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="78">
+        <v>5</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="C7" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" s="90">
-        <v>1.2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="D7" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="75">
+        <v>1.4</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="93">
-        <v>5</v>
-      </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="90">
-        <v>1.2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2787,145 +2859,209 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF8C125-206F-4B42-AF87-0D84A98FCE52}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" customWidth="1"/>
     <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="27"/>
+      <c r="A1" s="107"/>
       <c r="B1" s="27"/>
       <c r="C1" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="73"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="G7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="41">
+        <v>1</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C8" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="20" t="s">
+      <c r="D8" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="43">
+        <v>1</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="75" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="41">
+        <v>2</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="F9" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="43">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="90" t="s">
-        <v>117</v>
-      </c>
-      <c r="G8" s="44">
+      <c r="H9" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="108" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="41">
+        <v>3</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="109">
         <v>1</v>
       </c>
-      <c r="H8" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="90" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
-        <v>2</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="44">
+      <c r="H10" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="41">
+        <v>4</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="109">
         <v>1</v>
       </c>
-      <c r="H9" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="H11" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2968,83 +3104,83 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="21"/>
       <c r="D3" s="21"/>
       <c r="F3" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="23"/>
     </row>

</xml_diff>